<commit_message>
Customer and Address details
</commit_message>
<xml_diff>
--- a/docs/DB/JsonGenerator.xlsx
+++ b/docs/DB/JsonGenerator.xlsx
@@ -4,22 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="21075" windowHeight="8265"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="21075" windowHeight="8265" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="FoodItem" sheetId="1" r:id="rId1"/>
+    <sheet name="Address" sheetId="2" r:id="rId2"/>
+    <sheet name="Customer" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FoodItem!$A$1:$D$42</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="70">
   <si>
     <t>category</t>
   </si>
@@ -166,13 +166,76 @@
   </si>
   <si>
     <t>MAINS</t>
+  </si>
+  <si>
+    <t>line1</t>
+  </si>
+  <si>
+    <t>line2</t>
+  </si>
+  <si>
+    <t>line3</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>22/23 Feeder Road, Basanta Bihar</t>
+  </si>
+  <si>
+    <t>Belghoria</t>
+  </si>
+  <si>
+    <t>West Bengal</t>
+  </si>
+  <si>
+    <t>Kolkata</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Ranjan</t>
+  </si>
+  <si>
+    <t>Saha</t>
+  </si>
+  <si>
+    <t>ranjan.saha1@gmail.com</t>
+  </si>
+  <si>
+    <t>pinCode</t>
+  </si>
+  <si>
+    <t>_id</t>
+  </si>
+  <si>
+    <t>812c6c509441d38852dc3c4e</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>1991-12-04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +247,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -212,16 +283,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -523,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,24 +1253,143 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="116.140625" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2">
+        <v>700056</v>
+      </c>
+      <c r="H2" s="4" t="str">
+        <f>CONCATENATE("{""", $A$1, """:{""$oid"":""", A2, """},", """", $B$1, """:""", B2, """,""", $C$1, """:", IF(ISBLANK(C2), "null", CONCATENATE("""", C2, """")), ",""", $D$1, """:", IF(ISBLANK(D2), "null", CONCATENATE("""", D2, """")), ",""", $E$1, """:""", E2, """,""", $F$1, """:""", F2, """,""", $G$1, """:""", G2, """}")</f>
+        <v>{"_id":{"$oid":"812c6c509441d38852dc3c4e"},"line1":"22/23 Feeder Road, Basanta Bihar","line2":"Belghoria","line3":null,"state":"West Bengal","city":"Kolkata","pinCode":"700056"}</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="109.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2">
+        <v>9674467368</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="str">
+        <f>CONCATENATE("{""", $A$1, """:""", A2, """,""", $B$1, """:""", B2, """,""", $C$1, """:""", C2, """,""", $D$1, """:""", D2, """,""", $E$1, """", E2, """}")</f>
+        <v>{"firstName":"Ranjan","lastName":"Saha","phone":"9674467368","email":"ranjan.saha1@gmail.com","dob"1991-12-04"}</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>